<commit_message>
Fix CO2 Tax scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CO2_Tax.xlsx
+++ b/SuppXLS/Scen_SYS_CO2_Tax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAFC25F-55E2-4E4E-8F49-9053EB3679AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A67A9F6-F544-4405-A04C-BD63D0DB886A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INS" sheetId="2" r:id="rId1"/>
@@ -30,59 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Maurizio Gargiulo</author>
-    <author>Gary Goldstein</author>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Insert Table</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Define the qualifiers based upon commodity set + name + descriptions, according to both include and exclude specifications.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -126,21 +75,12 @@
     <t>Cset_CD</t>
   </si>
   <si>
-    <t>Attrib_Cond</t>
-  </si>
-  <si>
-    <t>Val_Cond</t>
-  </si>
-  <si>
     <t>Trans - Insert</t>
   </si>
   <si>
     <t>*CO2*,-*CO2S</t>
   </si>
   <si>
-    <t>CUR</t>
-  </si>
-  <si>
     <t>EUR19</t>
   </si>
   <si>
@@ -150,17 +90,26 @@
     <t>*CO2*</t>
   </si>
   <si>
-    <t>-T-A*INT*</t>
-  </si>
-  <si>
     <t>ENV</t>
+  </si>
+  <si>
+    <t>*,-T-A*INT*,-T-NAV*</t>
+  </si>
+  <si>
+    <t>Top_Check</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>CURR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,19 +139,6 @@
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -603,11 +539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,37 +552,38 @@
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -660,130 +597,135 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="I3" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="J3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>2020</v>
       </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4">
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
         <f>33.5/1000</f>
         <v>3.3500000000000002E-2</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>22</v>
+      <c r="J4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>20</v>
       </c>
       <c r="E5">
         <v>2030</v>
       </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5">
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5">
         <f>100/1000</f>
         <v>0.1</v>
       </c>
-      <c r="K5" t="str">
-        <f>K4</f>
-        <v>-T-A*INT*</v>
-      </c>
-      <c r="N5" t="str">
-        <f>N4</f>
+      <c r="J5" t="str">
+        <f>J4</f>
+        <v>*,-T-A*INT*,-T-NAV*</v>
+      </c>
+      <c r="M5" t="str">
+        <f>M4</f>
         <v>*CO2*</v>
       </c>
-      <c r="O5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P5" t="str">
-        <f>P4</f>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="str">
+        <f>O4</f>
         <v>*CO2*,-*CO2S</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="str">
+        <f>J5</f>
+        <v>*,-T-A*INT*,-T-NAV*</v>
+      </c>
+      <c r="M6" t="str">
+        <f>M5</f>
+        <v>*CO2*</v>
+      </c>
+      <c r="N6" t="s">
         <v>19</v>
       </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="K6" t="str">
-        <f>K5</f>
-        <v>-T-A*INT*</v>
-      </c>
-      <c r="N6" t="str">
-        <f>N5</f>
-        <v>*CO2*</v>
-      </c>
-      <c r="O6" t="s">
-        <v>23</v>
-      </c>
-      <c r="P6" t="str">
-        <f>P5</f>
+      <c r="O6" t="str">
+        <f>O5</f>
         <v>*CO2*,-*CO2S</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>